<commit_message>
alterações para salvar o plano de treino
</commit_message>
<xml_diff>
--- a/DOCUMENTOS/CRONOGRAMA/Cronograma_aplicativo_integrado_com_trello (Salvo automaticamente).xlsx
+++ b/DOCUMENTOS/CRONOGRAMA/Cronograma_aplicativo_integrado_com_trello (Salvo automaticamente).xlsx
@@ -12,14 +12,14 @@
     <sheet name="3 - Implementações" sheetId="4" r:id="rId3"/>
     <sheet name="4 - ROI" sheetId="3" r:id="rId4"/>
     <sheet name="5 -  Fluxo Principal" sheetId="5" r:id="rId5"/>
+    <sheet name="Fluxo_principal_detalhado" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="144525"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="55">
   <si>
     <t>PopUp ao excluir</t>
   </si>
@@ -163,6 +163,27 @@
   </si>
   <si>
     <t>Verificar todo o aplicativo e lançar todas as tarefas que faltam</t>
+  </si>
+  <si>
+    <t>Fazer o fluxo de cadastro de plano de treino completo</t>
+  </si>
+  <si>
+    <t>Fazer a listagem de plano de treinos</t>
+  </si>
+  <si>
+    <t>Nº</t>
+  </si>
+  <si>
+    <t>Descrição</t>
+  </si>
+  <si>
+    <t>Criar um serviço para sincronizar o plano de treino em caso de falha ao salvar.</t>
+  </si>
+  <si>
+    <t>Pegar o retorno da gravação do plano de treino, se não registrou, é preciso criar um serviço para sincronizar essa informação.</t>
+  </si>
+  <si>
+    <t>Terminar o processo de inclusão de plano de treino</t>
   </si>
 </sst>
 </file>
@@ -228,7 +249,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -236,11 +257,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -253,7 +289,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -740,7 +784,7 @@
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -860,8 +904,8 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>4</v>
+      <c r="A13" s="5" t="s">
+        <v>6</v>
       </c>
       <c r="B13" t="s">
         <v>23</v>
@@ -937,8 +981,8 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>4</v>
+      <c r="A20" s="5" t="s">
+        <v>6</v>
       </c>
       <c r="B20" t="s">
         <v>30</v>
@@ -1014,8 +1058,8 @@
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>4</v>
+      <c r="A27" s="5" t="s">
+        <v>6</v>
       </c>
       <c r="B27" t="s">
         <v>37</v>
@@ -1148,22 +1192,22 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D15" sqref="D14:G15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="58.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="58.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1171,7 +1215,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -1180,145 +1224,351 @@
       </c>
       <c r="E2" s="6">
         <f>SUM(C8:C1048576)</f>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6" s="6"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="C7" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="15">
+        <v>42461</v>
+      </c>
+      <c r="F7" s="15">
+        <v>42462</v>
+      </c>
+      <c r="G7" s="15">
+        <v>42463</v>
+      </c>
+      <c r="H7" s="15">
+        <v>42464</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="12">
         <v>1</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="B8" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="17">
+        <v>1</v>
+      </c>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="12">
         <v>2</v>
       </c>
-      <c r="D7" s="12">
-        <v>42461</v>
-      </c>
-      <c r="E7" s="12">
-        <v>42462</v>
-      </c>
-      <c r="F7" s="12">
-        <v>42463</v>
-      </c>
-      <c r="G7" s="12">
-        <v>42464</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="6">
+      <c r="B9" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="17">
+        <v>2</v>
+      </c>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="12">
+        <v>3</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="17">
+        <v>3</v>
+      </c>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="12">
+        <v>4</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="17">
+        <v>10</v>
+      </c>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="12">
+        <v>5</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="17"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="12">
+        <v>6</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="17"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
+        <v>7</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="12">
+        <v>8</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="6">
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="12">
+        <v>9</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="17">
+        <v>3</v>
+      </c>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="12">
+        <v>10</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="17"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="12">
+        <v>11</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="17"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="12">
+        <v>12</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="12">
+        <v>13</v>
+      </c>
+      <c r="B20" s="12"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="12">
+        <v>14</v>
+      </c>
+      <c r="B21" s="12"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="12">
+        <v>15</v>
+      </c>
+      <c r="B22" s="12"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="12">
+        <v>16</v>
+      </c>
+      <c r="B23" s="12"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="113.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>10</v>
+      </c>
+      <c r="B3">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" s="6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11" s="6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="B14" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" s="6">
-        <v>1</v>
-      </c>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B16" t="s">
-        <v>47</v>
-      </c>
-      <c r="C16" s="6">
-        <v>3</v>
+      <c r="C3" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>